<commit_message>
upload changes on ict ta
</commit_message>
<xml_diff>
--- a/_fmlReport.xlsx
+++ b/_fmlReport.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fas2020\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet1'!$A$1:$Q$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$Q$48</definedName>
   </definedNames>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>OFFICE</t>
   </si>
@@ -87,44 +92,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -132,10 +125,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="none"/>
@@ -148,27 +138,39 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -178,6 +180,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -192,81 +195,79 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -282,7 +283,7 @@
     <xdr:ext cx="1247775" cy="1200150"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 4" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -294,7 +295,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="0"/>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -312,7 +316,7 @@
     <xdr:ext cx="2943225" cy="809625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 6" descr=""/>
+        <xdr:cNvPr id="3" name="Picture 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -324,7 +328,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="0"/>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -342,7 +349,7 @@
     <xdr:ext cx="3419475" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr=""/>
+        <xdr:cNvPr id="4" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -354,37 +361,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="0"/>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="11430000" cy="1905000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="" descr=""/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="0"/>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -681,43 +661,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A9:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="160" view="pageLayout" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.7109375" customWidth="true" style="0"/>
-    <col min="7" max="7" width="15.28515625" customWidth="true" style="0"/>
-    <col min="8" max="8" width="16.7109375" customWidth="true" style="0"/>
-    <col min="9" max="9" width="10.85546875" customWidth="true" style="0"/>
-    <col min="10" max="10" width="13.42578125" customWidth="true" style="0"/>
-    <col min="11" max="11" width="16.7109375" customWidth="true" style="0"/>
-    <col min="15" max="15" width="9.85546875" customWidth="true" style="0"/>
-    <col min="16" max="16" width="10.85546875" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1"/>
-      <c r="M1"/>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="C2"/>
-    </row>
-    <row r="9" spans="1:17" customHeight="1" ht="14.45">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="12" t="s">
         <v>1</v>
       </c>
@@ -734,7 +706,7 @@
       <c r="P9" s="12"/>
       <c r="Q9" s="13"/>
     </row>
-    <row r="10" spans="1:17" customHeight="1" ht="14.45">
+    <row r="10" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -757,13 +729,13 @@
       <c r="P10" s="12"/>
       <c r="Q10" s="13"/>
     </row>
-    <row r="11" spans="1:17" customHeight="1" ht="14.45">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
@@ -780,83 +752,83 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="13" spans="1:17" customHeight="1" ht="14.45">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="11"/>
+      <c r="G13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17" t="s">
+      <c r="M13" s="15"/>
+      <c r="N13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="17"/>
-      <c r="P13" s="18" t="s">
+      <c r="O13" s="15"/>
+      <c r="P13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="Q13" s="15" t="s">
+      <c r="Q13" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:17" customHeight="1" ht="14.45">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="19" t="s">
+    <row r="14" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="20" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="20" t="s">
+      <c r="M14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="20" t="s">
+      <c r="N14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="O14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="15"/>
-    </row>
-    <row r="15" spans="1:17" customHeight="1" ht="14.45">
+      <c r="P14" s="11"/>
+      <c r="Q14" s="16"/>
+    </row>
+    <row r="15" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -875,7 +847,7 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" customHeight="1" ht="14.45">
+    <row r="16" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -894,7 +866,7 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -913,7 +885,7 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -932,7 +904,7 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -951,7 +923,7 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -970,7 +942,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -989,7 +961,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1008,7 +980,7 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1027,7 +999,7 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1046,7 +1018,7 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1065,7 +1037,7 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1084,7 +1056,7 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1103,7 +1075,7 @@
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1122,7 +1094,7 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1141,7 +1113,7 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1160,7 +1132,7 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1179,7 +1151,7 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1198,7 +1170,7 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1217,7 +1189,7 @@
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1236,7 +1208,7 @@
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1255,7 +1227,7 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1274,7 +1246,7 @@
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1293,7 +1265,7 @@
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1312,7 +1284,7 @@
       <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1331,7 +1303,7 @@
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1350,7 +1322,7 @@
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1369,7 +1341,7 @@
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1388,7 +1360,7 @@
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1407,7 +1379,7 @@
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1426,7 +1398,7 @@
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -1446,8 +1418,14 @@
       <c r="Q45" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="17">
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="E9:Q9"/>
     <mergeCell ref="E10:Q10"/>
@@ -1459,86 +1437,41 @@
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="I13:I14"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" scale="68" fitToHeight="0" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="48" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="17" man="1"/>
   </colBreaks>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>